<commit_message>
Error correction (Jeuk <> Puurs distance was wrong).
</commit_message>
<xml_diff>
--- a/Traveling Sam Problem.xlsx
+++ b/Traveling Sam Problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Projects/Traveling Sam Gooris Problem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725B8596-BE60-1F42-81B0-64517ECE077C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52120BC8-D62D-384C-9260-89D99FE9BAA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="460" windowWidth="27080" windowHeight="22180" activeTab="2" xr2:uid="{EA52A50A-5A7A-684D-81AF-6869E39545C4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="19180" activeTab="2" xr2:uid="{EA52A50A-5A7A-684D-81AF-6869E39545C4}"/>
   </bookViews>
   <sheets>
     <sheet name="ORIGINAL" sheetId="3" r:id="rId1"/>
@@ -43,10 +43,10 @@
     <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">9999999</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">300</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">600</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
@@ -58,7 +58,7 @@
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">9999999</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
@@ -67,7 +67,7 @@
     <definedName name="solver_opt" localSheetId="2" hidden="1">'Mere en Jeuk'!$AB$26</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">ORIGINAL!$AB$26</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
@@ -94,7 +94,7 @@
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">1000</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">600</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">600</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
@@ -916,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15878916-3C79-ED4D-BA35-ACFAC41031B1}">
   <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA26" sqref="AA26"/>
     </sheetView>
@@ -5423,9 +5423,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA063FF-6BB3-3945-B58C-44D2C6CD08AF}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA26" sqref="AA26"/>
+      <selection pane="bottomLeft" activeCell="AC15" sqref="AC15:AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5592,15 +5592,15 @@
       </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="20">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="AB2" s="5">
         <f>INDEX(CityDistance, AA25, AA2)</f>
-        <v>4.2</v>
+        <v>27.4</v>
       </c>
       <c r="AC2" s="25" t="str">
         <f>INDEX($A$2:$Y$25, AA2, 1)</f>
-        <v>Lint</v>
+        <v>Mere</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -5681,15 +5681,15 @@
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="21">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AB3" s="5">
         <f t="shared" ref="AB3:AB25" si="0">INDEX(CityDistance, AA2, AA3)</f>
-        <v>8.5</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="AC3" s="25" t="str">
         <f t="shared" ref="AC3:AC25" si="1">INDEX($A$2:$Y$25, AA3, 1)</f>
-        <v>Reet</v>
+        <v>Lot</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -5770,15 +5770,15 @@
       </c>
       <c r="Z4" s="1"/>
       <c r="AA4" s="21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AB4" s="5">
         <f t="shared" si="0"/>
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="AC4" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Niel</v>
+        <v>Vorst</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -5859,15 +5859,15 @@
       </c>
       <c r="Z5" s="1"/>
       <c r="AA5" s="21">
-        <v>23</v>
+        <v>14.999999999999998</v>
       </c>
       <c r="AB5" s="5">
         <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="AC5" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Boom</v>
+        <v>Jeuk</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -5948,15 +5948,15 @@
       </c>
       <c r="Z6" s="1"/>
       <c r="AA6" s="21">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="5">
         <f t="shared" si="0"/>
-        <v>37.6</v>
+        <v>29.8</v>
       </c>
       <c r="AC6" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Doel</v>
+        <v>Mal</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -6037,15 +6037,15 @@
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="21">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="AB7" s="5">
         <f t="shared" si="0"/>
-        <v>30.5</v>
+        <v>40.4</v>
       </c>
       <c r="AC7" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Sinnaai</v>
+        <v>As</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -6126,15 +6126,15 @@
       </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="21">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AB8" s="5">
         <f t="shared" si="0"/>
-        <v>67.5</v>
+        <v>15.7</v>
       </c>
       <c r="AC8" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Heist</v>
+        <v>Bree</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -6184,7 +6184,7 @@
         <v>68.400000000000006</v>
       </c>
       <c r="P9" s="4">
-        <v>37.200000000000003</v>
+        <v>97.2</v>
       </c>
       <c r="Q9" s="4">
         <v>46.2</v>
@@ -6215,15 +6215,15 @@
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="21">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="AB9" s="5">
         <f t="shared" si="0"/>
-        <v>54.7</v>
+        <v>10.7</v>
       </c>
       <c r="AC9" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Gits</v>
+        <v>Peer</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -6304,15 +6304,15 @@
       </c>
       <c r="Z10" s="1"/>
       <c r="AA10" s="21">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="AB10" s="5">
         <f t="shared" si="0"/>
-        <v>21.8</v>
+        <v>35.5</v>
       </c>
       <c r="AC10" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Tielt</v>
+        <v>Geel</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -6393,15 +6393,15 @@
       </c>
       <c r="Z11" s="1"/>
       <c r="AA11" s="21">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="AB11" s="5">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>33.5</v>
       </c>
       <c r="AC11" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Gent</v>
+        <v>Schriek</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -6482,15 +6482,15 @@
       </c>
       <c r="Z12" s="1"/>
       <c r="AA12" s="21">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AB12" s="5">
         <f t="shared" si="0"/>
-        <v>27.4</v>
+        <v>7.6</v>
       </c>
       <c r="AC12" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Mere</v>
+        <v>Haacht</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -6571,15 +6571,15 @@
       </c>
       <c r="Z13" s="1"/>
       <c r="AA13" s="21">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AB13" s="5">
         <f t="shared" si="0"/>
-        <v>40.200000000000003</v>
+        <v>23.6</v>
       </c>
       <c r="AC13" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Lot</v>
+        <v>Leest</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -6660,15 +6660,15 @@
       </c>
       <c r="Z14" s="1"/>
       <c r="AA14" s="21">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AB14" s="5">
         <f t="shared" si="0"/>
-        <v>6.7</v>
+        <v>12.4</v>
       </c>
       <c r="AC14" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Vorst</v>
+        <v>Duffel</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -6749,15 +6749,15 @@
       </c>
       <c r="Z15" s="1"/>
       <c r="AA15" s="21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AB15" s="5">
         <f t="shared" si="0"/>
-        <v>42.2</v>
+        <v>4.2</v>
       </c>
       <c r="AC15" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Puurs</v>
+        <v>Lint</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -6838,15 +6838,15 @@
       </c>
       <c r="Z16" s="1"/>
       <c r="AA16" s="21">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AB16" s="5">
         <f t="shared" si="0"/>
-        <v>37.200000000000003</v>
+        <v>8.5</v>
       </c>
       <c r="AC16" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Jeuk</v>
+        <v>Reet</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
@@ -6927,15 +6927,15 @@
       </c>
       <c r="Z17" s="1"/>
       <c r="AA17" s="21">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="AB17" s="5">
         <f t="shared" si="0"/>
-        <v>29.8</v>
+        <v>6.6</v>
       </c>
       <c r="AC17" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Mal</v>
+        <v>Niel</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
@@ -7016,15 +7016,15 @@
       </c>
       <c r="Z18" s="1"/>
       <c r="AA18" s="21">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="AB18" s="5">
         <f t="shared" si="0"/>
-        <v>40.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AC18" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>As</v>
+        <v>Boom</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
@@ -7105,15 +7105,15 @@
       </c>
       <c r="Z19" s="1"/>
       <c r="AA19" s="21">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AB19" s="5">
         <f t="shared" si="0"/>
-        <v>15.7</v>
+        <v>9.6</v>
       </c>
       <c r="AC19" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Bree</v>
+        <v>Puurs</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
@@ -7194,15 +7194,15 @@
       </c>
       <c r="Z20" s="1"/>
       <c r="AA20" s="21">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="AB20" s="5">
         <f t="shared" si="0"/>
-        <v>10.7</v>
+        <v>24.5</v>
       </c>
       <c r="AC20" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Peer</v>
+        <v>Sinnaai</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
@@ -7283,15 +7283,15 @@
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="21">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AB21" s="5">
         <f t="shared" si="0"/>
-        <v>35.5</v>
+        <v>30.6</v>
       </c>
       <c r="AC21" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Geel</v>
+        <v>Doel</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
@@ -7372,15 +7372,15 @@
       </c>
       <c r="Z22" s="1"/>
       <c r="AA22" s="21">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AB22" s="5">
         <f t="shared" si="0"/>
-        <v>33.5</v>
+        <v>85.3</v>
       </c>
       <c r="AC22" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Schriek</v>
+        <v>Heist</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
@@ -7461,15 +7461,15 @@
       </c>
       <c r="Z23" s="1"/>
       <c r="AA23" s="21">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AB23" s="5">
         <f t="shared" si="0"/>
-        <v>7.6</v>
+        <v>54.7</v>
       </c>
       <c r="AC23" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Haacht</v>
+        <v>Gits</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
@@ -7550,15 +7550,15 @@
       </c>
       <c r="Z24" s="1"/>
       <c r="AA24" s="21">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AB24" s="5">
         <f t="shared" si="0"/>
-        <v>23.6</v>
+        <v>21.8</v>
       </c>
       <c r="AC24" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Leest</v>
+        <v>Tielt</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7639,21 +7639,21 @@
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="21">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AB25" s="23">
         <f t="shared" si="0"/>
-        <v>12.4</v>
+        <v>34.5</v>
       </c>
       <c r="AC25" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>Duffel</v>
+        <v>Gent</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AB26" s="24">
         <f>SUM(AB2:AB25)</f>
-        <v>633.4</v>
+        <v>643.00000000000011</v>
       </c>
       <c r="AD26">
         <v>2025.6</v>

</xml_diff>